<commit_message>
Made improvements to layout and added silkscreen components.
This commit includes improvments to the physical layout as well as
comments on the silkscreen layer.
</commit_message>
<xml_diff>
--- a/eagle/Bill of Materials-v1.xlsx
+++ b/eagle/Bill of Materials-v1.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26519"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jonathan/GitHub/airU-bb/eagle/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16540" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="16540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -231,15 +236,6 @@
     <t>541-620FTR-ND</t>
   </si>
   <si>
-    <t>SMD 1206 1/4watt 449ohms 1% by Vishay</t>
-  </si>
-  <si>
-    <t>CRCW1206449RFKTA</t>
-  </si>
-  <si>
-    <t>71-CRCW12064490FT</t>
-  </si>
-  <si>
     <t>SMD 1206 1/4watt 62kohms 1% by Vishay</t>
   </si>
   <si>
@@ -265,6 +261,15 @@
   </si>
   <si>
     <t>Total Estimated Cost per Board</t>
+  </si>
+  <si>
+    <t>SMD 1206 1/4watt 453ohms 1% by Vishay</t>
+  </si>
+  <si>
+    <t>71-CRCW1206-453-E3</t>
+  </si>
+  <si>
+    <t>CRCW1206453RFKEA</t>
   </si>
 </sst>
 </file>
@@ -379,6 +384,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -707,10 +717,10 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
@@ -726,7 +736,7 @@
     <col min="12" max="12" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -756,7 +766,7 @@
       </c>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>7</v>
       </c>
@@ -786,7 +796,7 @@
         <v>3.698</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
         <v>36</v>
       </c>
@@ -816,7 +826,7 @@
         <v>9.9499999999999993</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>59</v>
       </c>
@@ -846,7 +856,7 @@
         <v>9.7200000000000006</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -864,7 +874,7 @@
         <v>29.95</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>26</v>
       </c>
@@ -894,7 +904,7 @@
         <v>1.2929999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>28</v>
       </c>
@@ -924,7 +934,7 @@
         <v>0.63700000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -954,7 +964,7 @@
         <v>1.82</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>33</v>
       </c>
@@ -984,7 +994,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>55</v>
       </c>
@@ -1014,7 +1024,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>23</v>
       </c>
@@ -1044,7 +1054,7 @@
         <v>1.492</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>42</v>
       </c>
@@ -1066,7 +1076,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>43</v>
       </c>
@@ -1096,7 +1106,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>47</v>
       </c>
@@ -1126,7 +1136,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>66</v>
       </c>
@@ -1156,18 +1166,18 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
@@ -1186,21 +1196,21 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="F20" t="s">
         <v>12</v>
@@ -1216,21 +1226,21 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="F21" t="s">
         <v>12</v>
@@ -1246,7 +1256,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>22</v>
       </c>
@@ -1276,7 +1286,7 @@
         <v>1.071</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>21</v>
       </c>
@@ -1306,7 +1316,7 @@
         <v>0.55300000000000005</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -1336,7 +1346,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>64</v>
       </c>
@@ -1350,9 +1360,9 @@
         <v>65</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B31" s="3">
         <f>SUM(I2:I26)+13</f>
@@ -1402,21 +1412,16 @@
     <hyperlink ref="C18" r:id="rId39"/>
     <hyperlink ref="D18" r:id="rId40"/>
     <hyperlink ref="E18" r:id="rId41"/>
-    <hyperlink ref="D19" r:id="rId42"/>
-    <hyperlink ref="C19" r:id="rId43"/>
-    <hyperlink ref="C20" r:id="rId44"/>
-    <hyperlink ref="D20" r:id="rId45"/>
-    <hyperlink ref="E20" r:id="rId46"/>
-    <hyperlink ref="C21" r:id="rId47"/>
-    <hyperlink ref="D21" r:id="rId48"/>
-    <hyperlink ref="E21" r:id="rId49"/>
+    <hyperlink ref="C20" r:id="rId42"/>
+    <hyperlink ref="D20" r:id="rId43"/>
+    <hyperlink ref="E20" r:id="rId44"/>
+    <hyperlink ref="C21" r:id="rId45"/>
+    <hyperlink ref="D21" r:id="rId46"/>
+    <hyperlink ref="E21" r:id="rId47"/>
+    <hyperlink ref="C19" r:id="rId48"/>
+    <hyperlink ref="D19" r:id="rId49"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>